<commit_message>
Cleaned up RDF Excel sample.
</commit_message>
<xml_diff>
--- a/tests/sample_files/sample_rdf.xlsx
+++ b/tests/sample_files/sample_rdf.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{DA3FDE2B-BE01-49EC-8AE4-4C9EB624C62F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BF969723-0F2A-46CC-94C6-F143809C8709}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2250" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2700" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="good" sheetId="1" r:id="rId1"/>
@@ -22,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
-  <si>
-    <t>h</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>foo</t>
   </si>
@@ -39,9 +36,6 @@
     <t>eggs</t>
   </si>
   <si>
-    <t>asdf</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -69,9 +63,6 @@
     <t>My Description</t>
   </si>
   <si>
-    <t>NO ELEMENT PROVIDED. THIS SHOULD NOT APPEAR IN THE RDF.</t>
-  </si>
-  <si>
     <t>My Relation</t>
   </si>
   <si>
@@ -82,6 +73,24 @@
   </si>
   <si>
     <t>identifier</t>
+  </si>
+  <si>
+    <t>extra_header</t>
+  </si>
+  <si>
+    <t>NO ELEMENT PROVIDED. THIS SHOULD BE IGNORED.</t>
+  </si>
+  <si>
+    <t>THIS SHOULD BE IGNORED.</t>
+  </si>
+  <si>
+    <t>id_1234</t>
+  </si>
+  <si>
+    <t>ignored</t>
+  </si>
+  <si>
+    <t>bad</t>
   </si>
 </sst>
 </file>
@@ -125,9 +134,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,82 +426,82 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="str">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="str">
         <f>CONCATENATE("My Type (this was created by Excel formula)")</f>
         <v>My Type (this was created by Excel formula)</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>15</v>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8">
-        <v>1234</v>
+        <v>16</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -499,47 +514,47 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -552,47 +567,47 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C12" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved worksheet name validation.
</commit_message>
<xml_diff>
--- a/tests/sample_files/sample_rdf.xlsx
+++ b/tests/sample_files/sample_rdf.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{268DC27C-19A3-4720-B8FB-963292374ADF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C80FCC8C-5B86-415B-9BD4-871927275039}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4050" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4500" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="good" sheetId="1" r:id="rId1"/>
-    <sheet name="good_too" sheetId="4" r:id="rId2"/>
+    <sheet name="good_2" sheetId="4" r:id="rId2"/>
     <sheet name="bad" sheetId="2" r:id="rId3"/>
     <sheet name="also_bad" sheetId="3" r:id="rId4"/>
   </sheets>
@@ -40,7 +40,7 @@
           <t>This worksheet is valid and will yield a METS &lt;dmdSec&gt; element if this file is passed to TOMES Packager.
 It is valid because it contains the valid headers "dc_element" and "dc_value".
 It is the user's responsibility to use correct Dublin Core element names in the "dc_element" column and legal XML values in the "dc_value" column.
-The name of the worksheet (e.g. "good") will be used for the &lt;dmdSec&gt; element's "ID" attribute value. Therefore, do not use whitespace or other illegal xml:id type values. Only use letters and underscores.
+The name of the worksheet (e.g. "good") will be used for the &lt;dmdSec&gt; element's "ID" attribute value. Use only letters, underscores, and numbers provided the name does not start with a number.
 Multiple worksheets within the same Excel file may be used. They will each yield a new METS &lt;dmdSec&gt; element.</t>
         </r>
       </text>

</xml_diff>